<commit_message>
[ADD] Flags tab for categories
</commit_message>
<xml_diff>
--- a/Flags.xlsx
+++ b/Flags.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Flags</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Somme positive</t>
   </si>
@@ -66,6 +63,45 @@
   </si>
   <si>
     <t>Somme négative Ventilée Rapprochée</t>
+  </si>
+  <si>
+    <t>Positif</t>
+  </si>
+  <si>
+    <t>Négatif</t>
+  </si>
+  <si>
+    <t>Rapproché</t>
+  </si>
+  <si>
+    <t>Rappel</t>
+  </si>
+  <si>
+    <t>Ventilé</t>
+  </si>
+  <si>
+    <t>Flags opérations</t>
+  </si>
+  <si>
+    <t>Flags Catégories</t>
+  </si>
+  <si>
+    <t>Dépense</t>
+  </si>
+  <si>
+    <t>Revenu</t>
+  </si>
+  <si>
+    <t>Possède un parent</t>
+  </si>
+  <si>
+    <t>Flags Ops</t>
+  </si>
+  <si>
+    <t>Possède une Op planifiée</t>
+  </si>
+  <si>
+    <t>Possède un budget</t>
   </si>
 </sst>
 </file>
@@ -383,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -395,108 +431,192 @@
     <col min="2" max="2" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>